<commit_message>
Tối ưu hoá thuật toán GA - Fix lỗi xác định không chính xác số tiết mỗi tuần
</commit_message>
<xml_diff>
--- a/timetabling_GA/results/HK2_CT01_2025/TKB_Hoc_Ky.xlsx
+++ b/timetabling_GA/results/HK2_CT01_2025/TKB_Hoc_Ky.xlsx
@@ -70,7 +70,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -81,6 +81,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="004A86E8"/>
         <bgColor rgb="004A86E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BDD7EE"/>
+        <bgColor rgb="00BDD7EE"/>
       </patternFill>
     </fill>
     <fill>
@@ -149,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -173,6 +179,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -651,16 +660,16 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7" t="n"/>
       <c r="E8" s="7" t="n"/>
@@ -668,10 +677,10 @@
       <c r="G8" s="7" t="n"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>MH004
-(Thực hành)
+          <t>MH003
+(Lý thuyết)
 Phòng: LT3
-GV: GV002</t>
+GV: GV007</t>
         </is>
       </c>
       <c r="I8" s="7" t="n"/>
@@ -680,43 +689,36 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C9" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7" t="n"/>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="9" t="inlineStr">
+        <is>
+          <t>MH004
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
+Phòng: TH3
+GV: GV002</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
@@ -734,55 +736,45 @@
       <c r="H10" s="8" t="inlineStr">
         <is>
           <t>MH003
-(Thực hành)
+(Lý thuyết)
 Phòng: LT3
-GV: GV007</t>
+GV: GV001</t>
         </is>
       </c>
       <c r="I10" s="7" t="n"/>
-      <c r="J10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J10" s="7" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="n"/>
       <c r="E11" s="7" t="n"/>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
       <c r="H11" s="7" t="n"/>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -795,7 +787,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -905,7 +897,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -916,18 +908,18 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
@@ -952,146 +944,74 @@
       <c r="H9" s="8" t="inlineStr">
         <is>
           <t>MH003
-(Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="n"/>
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="E10" s="7" t="n"/>
       <c r="F10" s="7" t="n"/>
       <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I10" s="7" t="n"/>
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="n"/>
       <c r="E11" s="7" t="n"/>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
+      <c r="H11" s="7" t="n"/>
+      <c r="I11" s="8" t="inlineStr">
         <is>
           <t>MH004
-(Thực hành)
-Phòng: TH1
+(Lý thuyết)
+Phòng: LT1
 GV: GV002</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
-      <c r="J13" s="7" t="n"/>
+      <c r="J11" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1104,7 +1024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1214,7 +1134,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1225,18 +1145,18 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
@@ -1261,146 +1181,74 @@
       <c r="H9" s="8" t="inlineStr">
         <is>
           <t>MH003
-(Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="n"/>
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="E10" s="7" t="n"/>
       <c r="F10" s="7" t="n"/>
       <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I10" s="7" t="n"/>
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="n"/>
       <c r="E11" s="7" t="n"/>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
+      <c r="H11" s="7" t="n"/>
+      <c r="I11" s="8" t="inlineStr">
         <is>
           <t>MH004
-(Thực hành)
-Phòng: TH1
+(Lý thuyết)
+Phòng: LT1
 GV: GV002</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
-      <c r="J13" s="7" t="n"/>
+      <c r="J11" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1413,7 +1261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1523,7 +1371,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1534,18 +1382,18 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
@@ -1570,146 +1418,74 @@
       <c r="H9" s="8" t="inlineStr">
         <is>
           <t>MH003
-(Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="n"/>
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="E10" s="7" t="n"/>
       <c r="F10" s="7" t="n"/>
       <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I10" s="7" t="n"/>
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="n"/>
       <c r="E11" s="7" t="n"/>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
+      <c r="H11" s="7" t="n"/>
+      <c r="I11" s="8" t="inlineStr">
         <is>
           <t>MH004
-(Thực hành)
-Phòng: TH1
+(Lý thuyết)
+Phòng: LT1
 GV: GV002</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
-      <c r="J13" s="7" t="n"/>
+      <c r="J11" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1722,7 +1498,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1832,7 +1608,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1843,18 +1619,18 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
@@ -1879,146 +1655,74 @@
       <c r="H9" s="8" t="inlineStr">
         <is>
           <t>MH003
-(Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="n"/>
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="E10" s="7" t="n"/>
       <c r="F10" s="7" t="n"/>
       <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I10" s="7" t="n"/>
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="n"/>
       <c r="E11" s="7" t="n"/>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
+      <c r="H11" s="7" t="n"/>
+      <c r="I11" s="8" t="inlineStr">
         <is>
           <t>MH004
-(Thực hành)
-Phòng: TH1
+(Lý thuyết)
+Phòng: LT1
 GV: GV002</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
-      <c r="J13" s="7" t="n"/>
+      <c r="J11" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2031,7 +1735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2141,7 +1845,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2152,18 +1856,18 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
@@ -2188,146 +1892,74 @@
       <c r="H9" s="8" t="inlineStr">
         <is>
           <t>MH003
-(Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="n"/>
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="E10" s="7" t="n"/>
       <c r="F10" s="7" t="n"/>
       <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I10" s="7" t="n"/>
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="n"/>
       <c r="E11" s="7" t="n"/>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
+      <c r="H11" s="7" t="n"/>
+      <c r="I11" s="8" t="inlineStr">
         <is>
           <t>MH004
-(Thực hành)
-Phòng: TH1
+(Lý thuyết)
+Phòng: LT1
 GV: GV002</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
-      <c r="J13" s="7" t="n"/>
+      <c r="J11" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2340,7 +1972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2450,7 +2082,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2461,18 +2093,18 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
@@ -2497,146 +2129,74 @@
       <c r="H9" s="8" t="inlineStr">
         <is>
           <t>MH003
-(Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="n"/>
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="E10" s="7" t="n"/>
       <c r="F10" s="7" t="n"/>
       <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I10" s="7" t="n"/>
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>DH23CS</t>
+          <t>L01</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="n"/>
       <c r="E11" s="7" t="n"/>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
+      <c r="H11" s="7" t="n"/>
+      <c r="I11" s="8" t="inlineStr">
         <is>
           <t>MH004
-(Thực hành)
-Phòng: TH1
+(Lý thuyết)
+Phòng: LT1
 GV: GV002</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
-      <c r="J13" s="7" t="n"/>
+      <c r="J11" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2649,7 +2209,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2759,60 +2319,31 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D8" s="7" t="n"/>
-      <c r="E8" s="8" t="inlineStr">
+        <v>30</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>MH004
-(Thực hành)
-Phòng: LT1
+(Lý thuyết)
+Phòng: LT3
 GV: GV002</t>
         </is>
       </c>
+      <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
       <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="n"/>
-      <c r="E9" s="7" t="n"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="G9" s="7" t="n"/>
-      <c r="H9" s="7" t="n"/>
-      <c r="I9" s="7" t="n"/>
-      <c r="J9" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2831,7 +2362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2941,7 +2472,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2952,27 +2483,23 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -2981,97 +2508,90 @@
       <c r="C9" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="n"/>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Thực hành)
+Phòng: TH2
+GV: GV007</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>MH004
+(Thực hành)
+Phòng: TH2
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="n"/>
+      <c r="J10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
+Phòng: TH1
+GV: GV007</t>
+        </is>
+      </c>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
+      <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -3088,45 +2608,75 @@
       <c r="G12" s="7" t="n"/>
       <c r="H12" s="7" t="n"/>
       <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
+      <c r="J12" s="9" t="inlineStr">
+        <is>
+          <t>MH004
 (Thực hành)
 Phòng: TH3
-GV: GV001</t>
+GV: GV002</t>
         </is>
       </c>
     </row>
     <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C13" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="n"/>
       <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
+      <c r="H13" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I13" s="7" t="n"/>
       <c r="J13" s="7" t="n"/>
     </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="10" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7" t="n"/>
+      <c r="E14" s="7" t="n"/>
+      <c r="F14" s="7" t="n"/>
+      <c r="G14" s="7" t="n"/>
+      <c r="H14" s="7" t="n"/>
+      <c r="I14" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="J14" s="7" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
@@ -3140,7 +2690,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3250,7 +2800,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3261,27 +2811,23 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -3290,97 +2836,90 @@
       <c r="C9" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="n"/>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Thực hành)
+Phòng: TH2
+GV: GV007</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>MH004
+(Thực hành)
+Phòng: TH2
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="n"/>
+      <c r="J10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
+Phòng: TH1
+GV: GV007</t>
+        </is>
+      </c>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
+      <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -3397,45 +2936,75 @@
       <c r="G12" s="7" t="n"/>
       <c r="H12" s="7" t="n"/>
       <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
+      <c r="J12" s="9" t="inlineStr">
+        <is>
+          <t>MH004
 (Thực hành)
 Phòng: TH3
-GV: GV001</t>
+GV: GV002</t>
         </is>
       </c>
     </row>
     <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C13" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="n"/>
       <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
+      <c r="H13" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I13" s="7" t="n"/>
       <c r="J13" s="7" t="n"/>
     </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="10" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7" t="n"/>
+      <c r="E14" s="7" t="n"/>
+      <c r="F14" s="7" t="n"/>
+      <c r="G14" s="7" t="n"/>
+      <c r="H14" s="7" t="n"/>
+      <c r="I14" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="J14" s="7" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
@@ -3449,7 +3018,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3559,7 +3128,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3570,27 +3139,23 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -3599,97 +3164,90 @@
       <c r="C9" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="n"/>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Thực hành)
+Phòng: TH2
+GV: GV007</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>MH004
+(Thực hành)
+Phòng: TH2
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="n"/>
+      <c r="J10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
+Phòng: TH1
+GV: GV007</t>
+        </is>
+      </c>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
+      <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -3706,45 +3264,75 @@
       <c r="G12" s="7" t="n"/>
       <c r="H12" s="7" t="n"/>
       <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
+      <c r="J12" s="9" t="inlineStr">
+        <is>
+          <t>MH004
 (Thực hành)
 Phòng: TH3
-GV: GV001</t>
+GV: GV002</t>
         </is>
       </c>
     </row>
     <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C13" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="n"/>
       <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
+      <c r="H13" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I13" s="7" t="n"/>
       <c r="J13" s="7" t="n"/>
     </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="10" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7" t="n"/>
+      <c r="E14" s="7" t="n"/>
+      <c r="F14" s="7" t="n"/>
+      <c r="G14" s="7" t="n"/>
+      <c r="H14" s="7" t="n"/>
+      <c r="I14" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="J14" s="7" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
@@ -3758,7 +3346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3868,7 +3456,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -3879,27 +3467,23 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -3908,97 +3492,90 @@
       <c r="C9" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="n"/>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Thực hành)
+Phòng: TH2
+GV: GV007</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>MH004
+(Thực hành)
+Phòng: TH2
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="n"/>
+      <c r="J10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
+Phòng: TH1
+GV: GV007</t>
+        </is>
+      </c>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
+      <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -4015,45 +3592,75 @@
       <c r="G12" s="7" t="n"/>
       <c r="H12" s="7" t="n"/>
       <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
+      <c r="J12" s="9" t="inlineStr">
+        <is>
+          <t>MH004
 (Thực hành)
 Phòng: TH3
-GV: GV001</t>
+GV: GV002</t>
         </is>
       </c>
     </row>
     <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>L01</t>
+          <t>DH23CS</t>
         </is>
       </c>
       <c r="C13" s="7" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="n"/>
       <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
+      <c r="H13" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I13" s="7" t="n"/>
       <c r="J13" s="7" t="n"/>
     </row>
+    <row r="14" ht="60" customHeight="1">
+      <c r="A14" s="10" t="n"/>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7" t="n"/>
+      <c r="E14" s="7" t="n"/>
+      <c r="F14" s="7" t="n"/>
+      <c r="G14" s="7" t="n"/>
+      <c r="H14" s="7" t="n"/>
+      <c r="I14" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="J14" s="7" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
@@ -4177,7 +3784,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -4188,27 +3795,23 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -4217,92 +3820,85 @@
       <c r="C9" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="n"/>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Thực hành)
+Phòng: TH2
+GV: GV007</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>MH004
+(Thực hành)
+Phòng: TH2
+GV: GV002</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="n"/>
+      <c r="J10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
+Phòng: TH1
+GV: GV007</t>
+        </is>
+      </c>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
+      <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
@@ -4322,19 +3918,19 @@
       <c r="E12" s="7" t="n"/>
       <c r="F12" s="7" t="n"/>
       <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
+      <c r="J12" s="7" t="n"/>
     </row>
     <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="10" t="n"/>
       <c r="B13" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -4345,21 +3941,22 @@
       </c>
       <c r="D13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="n"/>
       <c r="G13" s="7" t="n"/>
       <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
+      <c r="I13" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
       <c r="J13" s="7" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
@@ -4486,7 +4083,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -4497,27 +4094,23 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -4526,92 +4119,78 @@
       <c r="C9" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="n"/>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Thực hành)
+Phòng: TH2
+GV: GV007</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="7" t="n"/>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="n"/>
+      <c r="J10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
+Phòng: TH1
+GV: GV007</t>
+        </is>
+      </c>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
+      <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
@@ -4631,19 +4210,19 @@
       <c r="E12" s="7" t="n"/>
       <c r="F12" s="7" t="n"/>
       <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
+      <c r="J12" s="7" t="n"/>
     </row>
     <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="10" t="n"/>
       <c r="B13" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -4654,21 +4233,22 @@
       </c>
       <c r="D13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="n"/>
       <c r="G13" s="7" t="n"/>
       <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
+      <c r="I13" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
       <c r="J13" s="7" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
@@ -4795,7 +4375,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -4806,27 +4386,23 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -4835,92 +4411,78 @@
       <c r="C9" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="n"/>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Thực hành)
+Phòng: TH2
+GV: GV007</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="7" t="n"/>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="n"/>
+      <c r="J10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
+Phòng: TH1
+GV: GV007</t>
+        </is>
+      </c>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
+      <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
@@ -4940,19 +4502,19 @@
       <c r="E12" s="7" t="n"/>
       <c r="F12" s="7" t="n"/>
       <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
+      <c r="J12" s="7" t="n"/>
     </row>
     <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="10" t="n"/>
       <c r="B13" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -4963,21 +4525,22 @@
       </c>
       <c r="D13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="n"/>
       <c r="G13" s="7" t="n"/>
       <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
+      <c r="I13" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
       <c r="J13" s="7" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>
@@ -5104,7 +4667,7 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -5115,27 +4678,23 @@
       <c r="C8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT3
+GV: GV002</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="n"/>
       <c r="F8" s="7" t="n"/>
       <c r="G8" s="7" t="n"/>
-      <c r="H8" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT3
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
+      <c r="A9" s="10" t="n"/>
       <c r="B9" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -5144,92 +4703,78 @@
       <c r="C9" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="n"/>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH003
+(Thực hành)
+Phòng: TH2
+GV: GV007</t>
+        </is>
+      </c>
       <c r="E9" s="7" t="n"/>
       <c r="F9" s="7" t="n"/>
       <c r="G9" s="7" t="n"/>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="n"/>
+      <c r="I9" s="7" t="n"/>
+      <c r="J9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>L01</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="7" t="n"/>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV007</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="n"/>
+      <c r="J10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23CS</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>MH003
 (Thực hành)
-Phòng: TH2
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT1
-GV: GV001</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="n"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>L01</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: LT1
-GV: GV002</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23CS</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
+Phòng: TH1
+GV: GV007</t>
+        </is>
+      </c>
       <c r="F11" s="7" t="n"/>
       <c r="G11" s="7" t="n"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: LT3
-GV: GV007</t>
-        </is>
-      </c>
+      <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
-      <c r="J11" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH1
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
@@ -5249,19 +4794,19 @@
       <c r="E12" s="7" t="n"/>
       <c r="F12" s="7" t="n"/>
       <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>MH003
+(Lý thuyết)
+Phòng: LT3
+GV: GV001</t>
+        </is>
+      </c>
       <c r="I12" s="7" t="n"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <t>MH003
-(Thực hành)
-Phòng: TH3
-GV: GV001</t>
-        </is>
-      </c>
+      <c r="J12" s="7" t="n"/>
     </row>
     <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="9" t="n"/>
+      <c r="A13" s="10" t="n"/>
       <c r="B13" s="7" t="inlineStr">
         <is>
           <t>L01</t>
@@ -5272,21 +4817,22 @@
       </c>
       <c r="D13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>MH004
-(Thực hành)
-Phòng: TH2
-GV: GV002</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="n"/>
       <c r="G13" s="7" t="n"/>
       <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
+      <c r="I13" s="8" t="inlineStr">
+        <is>
+          <t>MH004
+(Lý thuyết)
+Phòng: LT1
+GV: GV002</t>
+        </is>
+      </c>
       <c r="J13" s="7" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A3:G3"/>

</xml_diff>